<commit_message>
add teaching guide for mear position
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.5.xlsx
+++ b/server/corelib/lang/all_lang_V1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C0C339-6F64-427F-A88F-0D44D221FDA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6704ECD-6F21-47A9-9736-F322D54899A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="1013">
   <si>
     <t>name</t>
   </si>
@@ -3184,6 +3184,127 @@
   </si>
   <si>
     <t>测试序列文件不存在！</t>
+  </si>
+  <si>
+    <t>seq_step</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>步驟</t>
+  </si>
+  <si>
+    <t>seq_sequence_teardown</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sequence Setup</t>
+  </si>
+  <si>
+    <t>seq_sequence_setup</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seq_enable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>seq_delete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schritt</t>
+  </si>
+  <si>
+    <t>步骤</t>
+  </si>
+  <si>
+    <t>流程準備程序</t>
+  </si>
+  <si>
+    <t>Sequenz-Setup</t>
+  </si>
+  <si>
+    <t>流程准备程序</t>
+  </si>
+  <si>
+    <t>Sequence Teardown</t>
+  </si>
+  <si>
+    <t>流程結束程序</t>
+  </si>
+  <si>
+    <t>Sequenz Teardown</t>
+  </si>
+  <si>
+    <t>流程结束程序</t>
+  </si>
+  <si>
+    <t>刪除</t>
+  </si>
+  <si>
+    <t>Löschen</t>
+  </si>
+  <si>
+    <t>open_teach_pos_pdf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Click me to open guide of teaching position</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击我打开教学位置指南</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Klicken Sie auf mich, um den Leitfaden für die Lehrposition zu öffnen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>點擊我打開教學位置指南</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>side_posteach</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>量測點教學</t>
+  </si>
+  <si>
+    <t>MearPos Führer</t>
+  </si>
+  <si>
+    <t>量测点教学</t>
+  </si>
+  <si>
+    <t>MearPos Guide</t>
+  </si>
+  <si>
+    <t>main_indicator_humidity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Humidity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>濕度</t>
+  </si>
+  <si>
+    <t>Feuchtigkeit</t>
+  </si>
+  <si>
+    <t>湿度</t>
   </si>
 </sst>
 </file>
@@ -3286,7 +3407,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4051,10 +4192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F214"/>
+  <dimension ref="A1:F222"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+      <selection activeCell="B207" sqref="B207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8184,377 +8325,547 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>936</v>
+        <v>1008</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>938</v>
+        <v>1009</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>940</v>
+        <v>1010</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>942</v>
+        <v>1011</v>
       </c>
       <c r="F207" s="4" t="s">
-        <v>943</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="F208" s="4" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>947</v>
+        <v>937</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>949</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>952</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>948</v>
-      </c>
-      <c r="F209" s="1" t="s">
-        <v>953</v>
+        <v>939</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>941</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="F209" s="4" t="s">
+        <v>945</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>959</v>
+        <v>946</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>958</v>
+        <v>951</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>961</v>
+        <v>950</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>962</v>
+        <v>955</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>965</v>
+        <v>958</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>967</v>
+        <v>960</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>968</v>
+        <v>961</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>967</v>
+        <v>962</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
+        <v>212</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
         <v>213</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="B215" s="1" t="s">
         <v>972</v>
       </c>
-      <c r="C214" s="1" t="s">
+      <c r="C215" s="1" t="s">
         <v>973</v>
       </c>
-      <c r="D214" s="1" t="s">
+      <c r="D215" s="1" t="s">
         <v>974</v>
       </c>
-      <c r="E214" s="1" t="s">
+      <c r="E215" s="1" t="s">
         <v>975</v>
       </c>
-      <c r="F214" s="1" t="s">
+      <c r="F215" s="1" t="s">
         <v>976</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>214</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>215</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>216</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>217</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>218</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>219</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>220</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>1006</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B167:E168 B1:E3 B153:E165 B96:E151 B69:E72 B5:E15 B75:E89 B17:E66 B177:E204 B207:E207 B209:E1048576">
+  <conditionalFormatting sqref="B167:E168 B1:E3 B153:E165 B96:E151 B69:E72 B5:E15 B75:E89 B17:E66 B177:E204 B208:E208 B210:E1048576">
+    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B166:E166">
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B169:E170">
     <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B166:E166">
+  <conditionalFormatting sqref="B152:E152">
     <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B169:E170">
+  <conditionalFormatting sqref="B171:E171 B172 D172:E172">
     <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B152:E152">
+  <conditionalFormatting sqref="B173:E173 B174 D174:E174">
     <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B171:E171 B172 D172:E172">
+  <conditionalFormatting sqref="B175:E176">
     <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B173:E173 B174 D174:E174">
+  <conditionalFormatting sqref="C174">
     <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B175:E176">
+  <conditionalFormatting sqref="C172">
     <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C174">
+  <conditionalFormatting sqref="B90:E90">
     <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C172">
+  <conditionalFormatting sqref="B91:D93">
     <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:E90">
+  <conditionalFormatting sqref="E91:E92">
     <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:D93">
+  <conditionalFormatting sqref="B94:D95">
     <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E92">
+  <conditionalFormatting sqref="E94:E95">
     <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:D95">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E94:E95">
+  <conditionalFormatting sqref="B67:E68">
     <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
+  <conditionalFormatting sqref="B205:E206">
     <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:E68">
+  <conditionalFormatting sqref="B73:D74">
     <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B205:E206">
+  <conditionalFormatting sqref="E74">
     <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:D74">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
+  <conditionalFormatting sqref="B16:E16">
     <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:E16">
+  <conditionalFormatting sqref="B204:E204">
     <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93">
+  <conditionalFormatting sqref="B203:E203">
     <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B204:E204">
+  <conditionalFormatting sqref="F167:F168 F1:F3 F153:F165 F96:F151 F69:F72 F5:F15 F75:F89 F17:F66 F177:F204 F208 F210:F1048576">
     <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B203:E203">
+  <conditionalFormatting sqref="F166">
     <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F167:F168 F1:F3 F153:F165 F96:F151 F69:F72 F5:F15 F75:F89 F17:F66 F177:F204 F207 F209:F1048576">
+  <conditionalFormatting sqref="F169:F170">
     <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F166">
+  <conditionalFormatting sqref="F152">
     <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F169:F170">
+  <conditionalFormatting sqref="F171:F172">
     <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F152">
+  <conditionalFormatting sqref="F173:F174">
     <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F171:F172">
+  <conditionalFormatting sqref="F175:F176">
     <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F173:F174">
+  <conditionalFormatting sqref="F90">
     <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F175:F176">
+  <conditionalFormatting sqref="F91:F93">
     <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90">
+  <conditionalFormatting sqref="F94:F95">
     <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:F93">
+  <conditionalFormatting sqref="F4">
     <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94:F95">
+  <conditionalFormatting sqref="F67:F68">
     <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="F205:F206">
     <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67:F68">
+  <conditionalFormatting sqref="F73:F74">
     <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F205:F206">
+  <conditionalFormatting sqref="F16">
     <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:F74">
+  <conditionalFormatting sqref="F204">
     <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
+  <conditionalFormatting sqref="F203">
     <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F204">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+  <conditionalFormatting sqref="B209:E209">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F203">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+  <conditionalFormatting sqref="F209">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B208:E208">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="B207:E207">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F208">
+  <conditionalFormatting sqref="F207">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>

<commit_message>
implemented circle define sample UI
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.5.xlsx
+++ b/server/corelib/lang/all_lang_V1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6704ECD-6F21-47A9-9736-F322D54899A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E007AFE-E777-4B35-A318-5E8C96A55D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="1018">
   <si>
     <t>name</t>
   </si>
@@ -1629,14 +1629,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>The Project and Batch are both exsisted! Do you want to continue this batch?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>此專案及批號已存在，是否要繼續?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>The batch is created successfully!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1887,9 +1879,6 @@
   </si>
   <si>
     <t>Datenbank verbunden</t>
-  </si>
-  <si>
-    <t>Das Projekt und Batch sind beide vorhanden! Möchten Sie die Bearbeitung fortsetzen?</t>
   </si>
   <si>
     <t>Batch existert</t>
@@ -2920,9 +2909,6 @@
     <t>连线至资料库成功</t>
   </si>
   <si>
-    <t>此专案及批号已存在，是否要继续?</t>
-  </si>
-  <si>
     <t>批号已存在</t>
   </si>
   <si>
@@ -3305,6 +3291,39 @@
   </si>
   <si>
     <t>湿度</t>
+  </si>
+  <si>
+    <t>server_reply_batch_seq_not_found</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The sequence file is not found</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>此測試流程檔案遺失</t>
+  </si>
+  <si>
+    <t>Die Sequenz-Datei nicht gefunden</t>
+  </si>
+  <si>
+    <t>此测试流程档案遗失</t>
+  </si>
+  <si>
+    <t>The Project and Batch {} are both exsisted! Do you want to continue this batch?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>此專案及批號 {} 已存在，是否要繼續?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Das Projekt und Batch {} sind beide vorhanden! Möchten Sie die Bearbeitung fortsetzen?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>此专案及批号 {} 已存在，是否要继续?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3407,7 +3426,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4192,10 +4231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F222"/>
+  <dimension ref="A1:F223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B207" sqref="B207"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4220,7 +4259,7 @@
         <v>320</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4240,7 +4279,7 @@
         <v>321</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4257,7 +4296,7 @@
         <v>113</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>113</v>
@@ -4268,19 +4307,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>614</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>615</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4300,7 +4339,7 @@
         <v>322</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4314,13 +4353,13 @@
         <v>115</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4334,13 +4373,13 @@
         <v>116</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4360,7 +4399,7 @@
         <v>117</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4368,7 +4407,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>118</v>
@@ -4388,7 +4427,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>119</v>
@@ -4420,7 +4459,7 @@
         <v>325</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4440,7 +4479,7 @@
         <v>321</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4460,7 +4499,7 @@
         <v>326</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4480,7 +4519,7 @@
         <v>327</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4488,7 +4527,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>123</v>
@@ -4508,19 +4547,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4540,7 +4579,7 @@
         <v>328</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4560,7 +4599,7 @@
         <v>328</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4580,7 +4619,7 @@
         <v>329</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4600,7 +4639,7 @@
         <v>329</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4620,7 +4659,7 @@
         <v>330</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4640,7 +4679,7 @@
         <v>330</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4660,7 +4699,7 @@
         <v>331</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4680,7 +4719,7 @@
         <v>332</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4700,7 +4739,7 @@
         <v>333</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4720,7 +4759,7 @@
         <v>334</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4740,7 +4779,7 @@
         <v>335</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4780,7 +4819,7 @@
         <v>133</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4800,7 +4839,7 @@
         <v>134</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4820,7 +4859,7 @@
         <v>337</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4837,10 +4876,10 @@
         <v>412</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4860,7 +4899,7 @@
         <v>338</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4880,7 +4919,7 @@
         <v>339</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4900,7 +4939,7 @@
         <v>340</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4920,7 +4959,7 @@
         <v>341</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4940,7 +4979,7 @@
         <v>342</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4960,7 +4999,7 @@
         <v>141</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -5000,7 +5039,7 @@
         <v>344</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -5020,7 +5059,7 @@
         <v>345</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -5040,7 +5079,7 @@
         <v>346</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -5060,7 +5099,7 @@
         <v>347</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -5080,7 +5119,7 @@
         <v>329</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -5120,7 +5159,7 @@
         <v>345</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -5160,7 +5199,7 @@
         <v>349</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -5177,10 +5216,10 @@
         <v>253</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -5200,7 +5239,7 @@
         <v>326</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -5220,7 +5259,7 @@
         <v>350</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -5260,7 +5299,7 @@
         <v>352</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -5280,7 +5319,7 @@
         <v>345</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -5300,7 +5339,7 @@
         <v>154</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -5337,10 +5376,10 @@
         <v>417</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -5360,7 +5399,7 @@
         <v>323</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -5377,10 +5416,10 @@
         <v>497</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5397,10 +5436,10 @@
         <v>470</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5417,10 +5456,10 @@
         <v>471</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -5437,10 +5476,10 @@
         <v>472</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5457,10 +5496,10 @@
         <v>473</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5477,10 +5516,10 @@
         <v>474</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5500,7 +5539,7 @@
         <v>334</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5517,10 +5556,10 @@
         <v>476</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5528,19 +5567,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -5548,19 +5587,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5577,10 +5616,10 @@
         <v>477</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -5597,10 +5636,10 @@
         <v>479</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -5617,10 +5656,10 @@
         <v>480</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -5637,10 +5676,10 @@
         <v>481</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -5648,19 +5687,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>715</v>
-      </c>
       <c r="D73" s="6" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
@@ -5668,19 +5707,19 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="D74" s="7" t="s">
         <v>713</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>717</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>716</v>
-      </c>
       <c r="E74" s="8" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -5697,10 +5736,10 @@
         <v>482</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -5717,10 +5756,10 @@
         <v>483</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -5737,10 +5776,10 @@
         <v>484</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -5748,19 +5787,19 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -5777,10 +5816,10 @@
         <v>485</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -5800,7 +5839,7 @@
         <v>157</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -5817,10 +5856,10 @@
         <v>487</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -5837,10 +5876,10 @@
         <v>488</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -5860,7 +5899,7 @@
         <v>331</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -5877,10 +5916,10 @@
         <v>490</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -5897,10 +5936,10 @@
         <v>491</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -5917,10 +5956,10 @@
         <v>492</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -5937,10 +5976,10 @@
         <v>493</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -5957,10 +5996,10 @@
         <v>494</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -5977,10 +6016,10 @@
         <v>495</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -5988,19 +6027,19 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -6008,19 +6047,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -6028,19 +6067,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="63" x14ac:dyDescent="0.25">
@@ -6048,19 +6087,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -6068,19 +6107,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>610</v>
-      </c>
       <c r="E94" s="1" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -6088,19 +6127,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>609</v>
-      </c>
       <c r="E95" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -6108,7 +6147,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>155</v>
@@ -6120,7 +6159,7 @@
         <v>353</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -6137,10 +6176,10 @@
         <v>259</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -6160,7 +6199,7 @@
         <v>157</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -6200,7 +6239,7 @@
         <v>355</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -6240,7 +6279,7 @@
         <v>357</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -6280,7 +6319,7 @@
         <v>359</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -6291,16 +6330,16 @@
         <v>57</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>524</v>
-      </c>
       <c r="F105" s="1" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -6320,7 +6359,7 @@
         <v>360</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -6340,7 +6379,7 @@
         <v>361</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -6360,7 +6399,7 @@
         <v>362</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -6380,7 +6419,7 @@
         <v>363</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -6400,7 +6439,7 @@
         <v>364</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -6420,7 +6459,7 @@
         <v>365</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -6440,7 +6479,7 @@
         <v>366</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -6460,7 +6499,7 @@
         <v>367</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -6480,7 +6519,7 @@
         <v>368</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -6500,7 +6539,7 @@
         <v>369</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -6520,7 +6559,7 @@
         <v>370</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -6580,7 +6619,7 @@
         <v>372</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -6600,7 +6639,7 @@
         <v>373</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -6640,7 +6679,7 @@
         <v>375</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -6660,7 +6699,7 @@
         <v>376</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -6680,7 +6719,7 @@
         <v>377</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -6700,7 +6739,7 @@
         <v>378</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -6717,10 +6756,10 @@
         <v>286</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -6740,7 +6779,7 @@
         <v>379</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -6760,7 +6799,7 @@
         <v>380</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -6780,7 +6819,7 @@
         <v>381</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -6800,7 +6839,7 @@
         <v>382</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -6820,7 +6859,7 @@
         <v>383</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -6840,7 +6879,7 @@
         <v>384</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -6860,7 +6899,7 @@
         <v>385</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -6880,7 +6919,7 @@
         <v>386</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -6900,7 +6939,7 @@
         <v>387</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -6920,7 +6959,7 @@
         <v>388</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -6940,7 +6979,7 @@
         <v>389</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -6960,7 +6999,7 @@
         <v>390</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -6977,7 +7016,7 @@
         <v>299</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>299</v>
@@ -7000,7 +7039,7 @@
         <v>391</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -7020,7 +7059,7 @@
         <v>392</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -7040,7 +7079,7 @@
         <v>393</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -7060,7 +7099,7 @@
         <v>394</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -7080,7 +7119,7 @@
         <v>395</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -7100,7 +7139,7 @@
         <v>396</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -7120,7 +7159,7 @@
         <v>397</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -7140,7 +7179,7 @@
         <v>398</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -7160,7 +7199,7 @@
         <v>399</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -7168,7 +7207,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>207</v>
@@ -7180,7 +7219,7 @@
         <v>400</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -7188,19 +7227,19 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D150" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="C150" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>531</v>
-      </c>
       <c r="E150" s="3" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -7208,19 +7247,19 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -7228,19 +7267,19 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="C152" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>534</v>
-      </c>
       <c r="E152" s="3" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -7260,7 +7299,7 @@
         <v>401</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -7280,7 +7319,7 @@
         <v>402</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -7300,7 +7339,7 @@
         <v>403</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -7320,7 +7359,7 @@
         <v>404</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -7340,7 +7379,7 @@
         <v>405</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -7360,7 +7399,7 @@
         <v>406</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -7380,7 +7419,7 @@
         <v>407</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -7400,7 +7439,7 @@
         <v>408</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -7420,7 +7459,7 @@
         <v>216</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -7440,7 +7479,7 @@
         <v>217</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -7457,10 +7496,10 @@
         <v>500</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F163" s="4" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -7477,10 +7516,10 @@
         <v>503</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F164" s="4" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -7488,19 +7527,19 @@
         <v>164</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>504</v>
+        <v>1014</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>505</v>
+        <v>1015</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>577</v>
+        <v>1016</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>896</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -7508,19 +7547,19 @@
         <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D166" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="C166" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>514</v>
-      </c>
       <c r="E166" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -7528,19 +7567,19 @@
         <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -7548,779 +7587,779 @@
         <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C168" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="D168" s="1" t="s">
-        <v>515</v>
-      </c>
       <c r="E168" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>516</v>
+        <v>1009</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>518</v>
+        <v>1010</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>520</v>
+        <v>1011</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>581</v>
+        <v>1012</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>900</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>538</v>
+        <v>519</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>902</v>
+        <v>897</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D172" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>539</v>
-      </c>
       <c r="E172" s="1" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>760</v>
+        <v>534</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>542</v>
+        <v>586</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B174" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="C174" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>589</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>539</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="D175" s="6" t="s">
+        <v>586</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="E175" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="E175" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="F175" s="6" t="s">
-        <v>905</v>
+      <c r="F175" s="1" t="s">
+        <v>899</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>539</v>
+        <v>584</v>
+      </c>
+      <c r="D176" s="6" t="s">
+        <v>582</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="F176" s="1" t="s">
-        <v>903</v>
+        <v>583</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>901</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>176</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>626</v>
+        <v>175</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>542</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>650</v>
+        <v>586</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>651</v>
+        <v>537</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>732</v>
+        <v>585</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>697</v>
+        <v>623</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>627</v>
+        <v>694</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>911</v>
+        <v>906</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>933</v>
+        <v>630</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>915</v>
+        <v>910</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>634</v>
+        <v>929</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>916</v>
+        <v>911</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>699</v>
+        <v>668</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>559</v>
+        <v>741</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>818</v>
+        <v>914</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>745</v>
+        <v>557</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>919</v>
+        <v>815</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>677</v>
+        <v>699</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>921</v>
+        <v>916</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>922</v>
+        <v>917</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>703</v>
+        <v>678</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>923</v>
+        <v>918</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>684</v>
+        <v>700</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>924</v>
+        <v>919</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>685</v>
+        <v>747</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>824</v>
+        <v>920</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>751</v>
+        <v>684</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>925</v>
+        <v>822</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>693</v>
+        <v>749</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>927</v>
+        <v>922</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>753</v>
+        <v>690</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>928</v>
+        <v>923</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>935</v>
+        <v>646</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="D203" s="6" t="s">
-        <v>756</v>
-      </c>
-      <c r="E203" s="3" t="s">
-        <v>758</v>
-      </c>
-      <c r="F203" s="6" t="s">
-        <v>931</v>
+        <v>692</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>924</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="D204" s="4" t="s">
-        <v>757</v>
+        <v>752</v>
+      </c>
+      <c r="D204" s="6" t="s">
+        <v>753</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>759</v>
-      </c>
-      <c r="F204" s="4" t="s">
-        <v>932</v>
+        <v>755</v>
+      </c>
+      <c r="F204" s="6" t="s">
+        <v>927</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>705</v>
+        <v>930</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>458</v>
+        <v>751</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>706</v>
+        <v>754</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>711</v>
+        <v>756</v>
       </c>
       <c r="F205" s="4" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E206" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="F206" s="4" t="s">
-        <v>930</v>
+        <v>925</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -8328,544 +8367,574 @@
         <v>205</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>1008</v>
+        <v>701</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>1009</v>
+        <v>457</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>1010</v>
+        <v>704</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>1011</v>
+        <v>706</v>
       </c>
       <c r="F207" s="4" t="s">
-        <v>1012</v>
+        <v>926</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>936</v>
+        <v>1004</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>938</v>
+        <v>1005</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>940</v>
+        <v>1006</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>942</v>
+        <v>1007</v>
       </c>
       <c r="F208" s="4" t="s">
-        <v>943</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="C209" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="F209" s="4" t="s">
         <v>939</v>
-      </c>
-      <c r="D209" s="4" t="s">
-        <v>941</v>
-      </c>
-      <c r="E209" s="3" t="s">
-        <v>944</v>
-      </c>
-      <c r="F209" s="4" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>947</v>
+        <v>933</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>949</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>952</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>948</v>
-      </c>
-      <c r="F210" s="1" t="s">
-        <v>953</v>
+        <v>935</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="F210" s="4" t="s">
+        <v>941</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>951</v>
+        <v>945</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>950</v>
+        <v>944</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>959</v>
+        <v>942</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>958</v>
+        <v>947</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>960</v>
+        <v>950</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>961</v>
+        <v>946</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>962</v>
+        <v>951</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>965</v>
+        <v>954</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>967</v>
+        <v>956</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>968</v>
+        <v>957</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>967</v>
+        <v>958</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B214" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E214" s="1" t="s">
         <v>964</v>
       </c>
-      <c r="C214" s="1" t="s">
-        <v>966</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>969</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>970</v>
-      </c>
       <c r="F214" s="1" t="s">
-        <v>971</v>
+        <v>963</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>972</v>
+        <v>960</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>973</v>
+        <v>962</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>974</v>
+        <v>965</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>975</v>
+        <v>966</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>977</v>
+        <v>968</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>978</v>
+        <v>969</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>979</v>
+        <v>970</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>987</v>
+        <v>971</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>988</v>
+        <v>972</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>982</v>
+        <v>973</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>981</v>
+        <v>974</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>989</v>
+        <v>975</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>990</v>
+        <v>983</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>991</v>
+        <v>984</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>992</v>
+        <v>977</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>993</v>
+        <v>985</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>994</v>
+        <v>986</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>995</v>
+        <v>987</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>983</v>
+        <v>976</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>984</v>
+        <v>988</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>248</v>
+        <v>989</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>346</v>
+        <v>990</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>792</v>
+        <v>991</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>986</v>
+        <v>979</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>985</v>
+        <v>980</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>996</v>
+        <v>248</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>997</v>
+        <v>346</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>809</v>
+        <v>789</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>998</v>
+        <v>982</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>999</v>
+        <v>981</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1002</v>
+        <v>992</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>1001</v>
+        <v>993</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>1000</v>
+        <v>806</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
+        <v>219</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
         <v>220</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B223" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="C223" s="1" t="s">
         <v>1003</v>
       </c>
-      <c r="C222" s="1" t="s">
-        <v>1007</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>1004</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F222" s="1" t="s">
-        <v>1006</v>
+      <c r="D223" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>1002</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B167:E168 B1:E3 B153:E165 B96:E151 B69:E72 B5:E15 B75:E89 B17:E66 B177:E204 B208:E208 B210:E1048576">
+  <conditionalFormatting sqref="B167:E168 B1:E3 B153:E165 B96:E151 B69:E72 B5:E15 B75:E89 B17:E66 B178:E205 B209:E209 B211:E1048576">
+    <cfRule type="cellIs" dxfId="46" priority="49" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B166:E166">
+    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B170:E171">
     <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B166:E166">
+  <conditionalFormatting sqref="B152:E152">
     <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B169:E170">
+  <conditionalFormatting sqref="B172:E172 B173 D173:E173">
     <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B152:E152">
+  <conditionalFormatting sqref="B174:E174 B175 D175:E175">
     <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B171:E171 B172 D172:E172">
+  <conditionalFormatting sqref="B176:E177">
     <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B173:E173 B174 D174:E174">
+  <conditionalFormatting sqref="C175">
     <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B175:E176">
+  <conditionalFormatting sqref="C173">
     <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C174">
+  <conditionalFormatting sqref="B90:E90">
     <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C172">
+  <conditionalFormatting sqref="B91:D93">
     <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:E90">
+  <conditionalFormatting sqref="E91:E92">
     <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:D93">
+  <conditionalFormatting sqref="B94:D95">
     <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E92">
+  <conditionalFormatting sqref="E94:E95">
     <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:D95">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E94:E95">
+  <conditionalFormatting sqref="B67:E68">
     <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
+  <conditionalFormatting sqref="B206:E207">
     <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:E68">
+  <conditionalFormatting sqref="B73:D74">
     <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B205:E206">
+  <conditionalFormatting sqref="E74">
     <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:D74">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
+  <conditionalFormatting sqref="B16:E16">
     <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:E16">
+  <conditionalFormatting sqref="B205:E205">
     <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93">
+  <conditionalFormatting sqref="B204:E204">
     <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B204:E204">
+  <conditionalFormatting sqref="F167:F168 F1:F3 F153:F165 F96:F151 F69:F72 F5:F15 F75:F89 F17:F66 F178:F205 F209 F211:F1048576">
     <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B203:E203">
+  <conditionalFormatting sqref="F166">
     <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F167:F168 F1:F3 F153:F165 F96:F151 F69:F72 F5:F15 F75:F89 F17:F66 F177:F204 F208 F210:F1048576">
+  <conditionalFormatting sqref="F170:F171">
     <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F166">
+  <conditionalFormatting sqref="F152">
     <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F169:F170">
+  <conditionalFormatting sqref="F172:F173">
     <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F152">
+  <conditionalFormatting sqref="F174:F175">
     <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F171:F172">
+  <conditionalFormatting sqref="F176:F177">
     <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F173:F174">
+  <conditionalFormatting sqref="F90">
     <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F175:F176">
+  <conditionalFormatting sqref="F91:F93">
     <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90">
+  <conditionalFormatting sqref="F94:F95">
     <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:F93">
+  <conditionalFormatting sqref="F4">
     <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94:F95">
+  <conditionalFormatting sqref="F67:F68">
     <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="F206:F207">
     <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67:F68">
+  <conditionalFormatting sqref="F73:F74">
     <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F205:F206">
+  <conditionalFormatting sqref="F16">
     <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:F74">
+  <conditionalFormatting sqref="F205">
     <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
+  <conditionalFormatting sqref="F204">
     <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F204">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+  <conditionalFormatting sqref="B210:E210">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F203">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+  <conditionalFormatting sqref="F210">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B209:E209">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+  <conditionalFormatting sqref="B208:E208">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F209">
+  <conditionalFormatting sqref="F208">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B207:E207">
+  <conditionalFormatting sqref="B169:E169">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207">
+  <conditionalFormatting sqref="F169">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>

<commit_message>
implemented sample monitor UI
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.5.xlsx
+++ b/server/corelib/lang/all_lang_V1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E007AFE-E777-4B35-A318-5E8C96A55D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A1B674-5247-4741-977E-1C081CDAE5A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="1055">
   <si>
     <t>name</t>
   </si>
@@ -3324,6 +3324,140 @@
   <si>
     <t>此专案及批号 {} 已存在，是否要继续?</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>run_stauts_monitor_title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample Monitor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>樣品即時監測</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>run_open_sampleSetupList_btn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Setup</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試設定</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modal_batch_setup_dialog_title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sampleBatchConfigAdd_btn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sampleBatchConfigClearAll_btn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clear All Samples</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除所有樣品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveLastBtn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveHomeBtn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveNextBtn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>To Home</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>To Last Position</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>To Next Position</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>移動至下個位置</t>
+  </si>
+  <si>
+    <t>移動至上個位置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>回原點</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Probe-Monitor</t>
+  </si>
+  <si>
+    <t>样品即时监测</t>
+  </si>
+  <si>
+    <t>Versuchsaufbau</t>
+  </si>
+  <si>
+    <t>测试设定</t>
+  </si>
+  <si>
+    <t>Alle Proben</t>
+  </si>
+  <si>
+    <t>清除所有样品</t>
+  </si>
+  <si>
+    <t>Letzte Position</t>
+  </si>
+  <si>
+    <t>移动至上个位置</t>
+  </si>
+  <si>
+    <t>Nach Hause</t>
+  </si>
+  <si>
+    <t>回原点</t>
+  </si>
+  <si>
+    <t>Zum nächsten Position</t>
+  </si>
+  <si>
+    <t>移动至下个位置</t>
+  </si>
+  <si>
+    <t>sampleSetupConfirmBtn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>確定</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定</t>
   </si>
 </sst>
 </file>
@@ -4231,10 +4365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F223"/>
+  <dimension ref="A1:F232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E232" sqref="E232:F232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8700,6 +8834,183 @@
       </c>
       <c r="F223" s="1" t="s">
         <v>1002</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>221</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D224" s="6" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>222</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>223</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>224</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>225</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>226</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>227</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>228</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B232" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>1054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the rotation bug; remove go next and last; replace with go index
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.5.xlsx
+++ b/server/corelib/lang/all_lang_V1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F79D1D-3D24-48C5-BE1E-6D91A6FD1A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC4DBDF-13F4-4409-962F-CA1749E94D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="1065">
   <si>
     <t>name</t>
   </si>
@@ -3474,6 +3474,23 @@
   </si>
   <si>
     <t>sampleBatchConfigClearAllBtn</t>
+  </si>
+  <si>
+    <t>goToIndexBtn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Go To Index</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zur Index</t>
+  </si>
+  <si>
+    <t>转至索引位置</t>
+  </si>
+  <si>
+    <t>轉至索引位置</t>
   </si>
 </sst>
 </file>
@@ -4381,10 +4398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F233"/>
+  <dimension ref="A1:F234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D230" sqref="D230"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B231" sqref="B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9050,6 +9067,26 @@
       </c>
       <c r="F233" s="1" t="s">
         <v>1046</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>232</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>1063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemened manual and auto mode switch
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.5.xlsx
+++ b/server/corelib/lang/all_lang_V1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC4DBDF-13F4-4409-962F-CA1749E94D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B748E294-A127-46AA-A76B-C3B2964C933D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="1070">
   <si>
     <t>name</t>
   </si>
@@ -2383,9 +2383,6 @@
   &lt;h3&gt;Betätige &lt;strong&gt;Nächster Schritt&lt;/strong&gt; um an nächster Position zu messen!&lt;/h3&gt;</t>
   </si>
   <si>
-    <t>Proben ID</t>
-  </si>
-  <si>
     <t>Messdaten</t>
   </si>
   <si>
@@ -3491,6 +3488,27 @@
   </si>
   <si>
     <t>轉至索引位置</t>
+  </si>
+  <si>
+    <t>modal_moving_sample_sampleIndex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample Index</t>
+  </si>
+  <si>
+    <t>Sample Index</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>該批號內之待測物流水號</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proben-ID</t>
+  </si>
+  <si>
+    <t>该批号内之待测物流水号</t>
   </si>
 </sst>
 </file>
@@ -3593,7 +3611,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4398,10 +4446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F234"/>
+  <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B231" sqref="B231"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4426,7 +4474,7 @@
         <v>320</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4446,7 +4494,7 @@
         <v>321</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4486,7 +4534,7 @@
         <v>607</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4506,7 +4554,7 @@
         <v>322</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4526,7 +4574,7 @@
         <v>540</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4546,7 +4594,7 @@
         <v>596</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4566,7 +4614,7 @@
         <v>117</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4574,7 +4622,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>118</v>
@@ -4594,7 +4642,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>119</v>
@@ -4626,7 +4674,7 @@
         <v>325</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4646,7 +4694,7 @@
         <v>321</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4666,7 +4714,7 @@
         <v>326</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4686,7 +4734,7 @@
         <v>327</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4726,7 +4774,7 @@
         <v>712</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4746,7 +4794,7 @@
         <v>328</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4766,7 +4814,7 @@
         <v>328</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4786,7 +4834,7 @@
         <v>329</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4806,7 +4854,7 @@
         <v>329</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4826,7 +4874,7 @@
         <v>330</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4846,7 +4894,7 @@
         <v>330</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4866,7 +4914,7 @@
         <v>331</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4886,7 +4934,7 @@
         <v>332</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4906,7 +4954,7 @@
         <v>333</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4926,7 +4974,7 @@
         <v>334</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4946,7 +4994,7 @@
         <v>335</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4986,7 +5034,7 @@
         <v>133</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -5006,7 +5054,7 @@
         <v>134</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5026,7 +5074,7 @@
         <v>337</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -5046,7 +5094,7 @@
         <v>541</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -5066,7 +5114,7 @@
         <v>338</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -5086,7 +5134,7 @@
         <v>339</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -5106,7 +5154,7 @@
         <v>340</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -5126,7 +5174,7 @@
         <v>341</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -5146,7 +5194,7 @@
         <v>342</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -5166,7 +5214,7 @@
         <v>141</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -5206,7 +5254,7 @@
         <v>344</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,7 +5274,7 @@
         <v>345</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -5246,7 +5294,7 @@
         <v>346</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -5266,7 +5314,7 @@
         <v>347</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5334,7 @@
         <v>329</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -5326,7 +5374,7 @@
         <v>345</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -5366,7 +5414,7 @@
         <v>349</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -5386,7 +5434,7 @@
         <v>542</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -5406,7 +5454,7 @@
         <v>326</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -5426,7 +5474,7 @@
         <v>350</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -5466,7 +5514,7 @@
         <v>352</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -5486,7 +5534,7 @@
         <v>345</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -5506,7 +5554,7 @@
         <v>154</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -5546,7 +5594,7 @@
         <v>544</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -5566,7 +5614,7 @@
         <v>323</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -5586,7 +5634,7 @@
         <v>543</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5606,7 +5654,7 @@
         <v>700</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5626,7 +5674,7 @@
         <v>702</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -5646,7 +5694,7 @@
         <v>545</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5666,7 +5714,7 @@
         <v>546</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5686,7 +5734,7 @@
         <v>547</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5706,7 +5754,7 @@
         <v>334</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5726,7 +5774,7 @@
         <v>548</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5746,7 +5794,7 @@
         <v>614</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -5766,7 +5814,7 @@
         <v>615</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5786,7 +5834,7 @@
         <v>549</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -5806,7 +5854,7 @@
         <v>550</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -5826,7 +5874,7 @@
         <v>551</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -5846,7 +5894,7 @@
         <v>552</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -5866,7 +5914,7 @@
         <v>715</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
@@ -5886,7 +5934,7 @@
         <v>716</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -5906,7 +5954,7 @@
         <v>553</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -5926,7 +5974,7 @@
         <v>556</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -5946,7 +5994,7 @@
         <v>554</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -5966,7 +6014,7 @@
         <v>717</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -5986,7 +6034,7 @@
         <v>555</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -6006,7 +6054,7 @@
         <v>157</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -6026,7 +6074,7 @@
         <v>557</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -6046,7 +6094,7 @@
         <v>558</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -6066,7 +6114,7 @@
         <v>331</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -6086,7 +6134,7 @@
         <v>559</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -6106,7 +6154,7 @@
         <v>560</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -6126,7 +6174,7 @@
         <v>561</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -6146,7 +6194,7 @@
         <v>562</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -6157,16 +6205,16 @@
         <v>454</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>493</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -6177,16 +6225,16 @@
         <v>455</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -6206,7 +6254,7 @@
         <v>718</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -6226,7 +6274,7 @@
         <v>719</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -6246,7 +6294,7 @@
         <v>720</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="63" x14ac:dyDescent="0.25">
@@ -6266,7 +6314,7 @@
         <v>721</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -6274,1499 +6322,1499 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>597</v>
+        <v>1064</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>599</v>
+        <v>1066</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>602</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>722</v>
+        <v>1065</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>601</v>
+        <v>1067</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>723</v>
+        <v>1068</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>826</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>582</v>
+        <v>598</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>258</v>
+        <v>600</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>601</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>827</v>
+        <v>722</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>825</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>49</v>
+        <v>582</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>555</v>
+        <v>353</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>812</v>
+        <v>826</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>157</v>
+        <v>555</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>354</v>
+        <v>157</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>251</v>
+        <v>812</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>828</v>
+        <v>251</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>262</v>
+        <v>827</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>829</v>
+        <v>262</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>264</v>
+        <v>828</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>830</v>
+        <v>264</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>517</v>
+        <v>163</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>518</v>
+        <v>265</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>519</v>
+        <v>359</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>164</v>
+        <v>517</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>266</v>
+        <v>518</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>360</v>
+        <v>519</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>175</v>
+        <v>370</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>277</v>
+        <v>841</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>371</v>
+        <v>175</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>843</v>
+        <v>278</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>281</v>
+        <v>843</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>845</v>
+        <v>281</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>563</v>
+        <v>378</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>379</v>
+        <v>563</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>564</v>
+        <v>390</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>299</v>
+        <v>860</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>391</v>
+        <v>564</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>862</v>
+        <v>299</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>522</v>
+        <v>100</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>525</v>
+        <v>207</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="E150" s="3" t="s">
-        <v>565</v>
+        <v>309</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>400</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>101</v>
+        <v>527</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>208</v>
+        <v>528</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>401</v>
+        <v>529</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>567</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>216</v>
+        <v>408</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>495</v>
+        <v>110</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="D163" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="E163" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="F163" s="4" t="s">
-        <v>885</v>
+        <v>217</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F164" s="4" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>164</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>506</v>
+        <v>163</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>498</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>1008</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>1011</v>
+        <v>499</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="F165" s="4" t="s">
+        <v>885</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>505</v>
+        <v>1007</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>509</v>
+        <v>1008</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>570</v>
+        <v>1009</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>887</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -7774,136 +7822,136 @@
         <v>167</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1003</v>
+        <v>504</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>1004</v>
+        <v>508</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1005</v>
+        <v>510</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>1006</v>
+        <v>572</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>1007</v>
+        <v>888</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>511</v>
+        <v>1002</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>513</v>
+        <v>1003</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>515</v>
+        <v>1004</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>573</v>
+        <v>1005</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>890</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>530</v>
+        <v>512</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>532</v>
+        <v>514</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>581</v>
+        <v>532</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>752</v>
+        <v>531</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>537</v>
+        <v>581</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>535</v>
+        <v>751</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>581</v>
+        <v>537</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>893</v>
@@ -7911,607 +7959,607 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="D176" s="6" t="s">
-        <v>577</v>
+        <v>581</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>534</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="F176" s="6" t="s">
-        <v>895</v>
+        <v>580</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>892</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>534</v>
+        <v>579</v>
+      </c>
+      <c r="D177" s="6" t="s">
+        <v>577</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>893</v>
+        <v>578</v>
+      </c>
+      <c r="F177" s="6" t="s">
+        <v>894</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>176</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>618</v>
+        <v>175</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>539</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>642</v>
+        <v>581</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>643</v>
+        <v>534</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>724</v>
+        <v>580</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>689</v>
+        <v>618</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>619</v>
+        <v>689</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>923</v>
+        <v>625</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>626</v>
+        <v>922</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>691</v>
+        <v>663</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>554</v>
+        <v>735</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>810</v>
+        <v>907</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>737</v>
+        <v>554</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>909</v>
+        <v>809</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>669</v>
+        <v>694</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1053</v>
+        <v>631</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>1054</v>
+        <v>668</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>1055</v>
+        <v>669</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>1056</v>
+        <v>737</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>1057</v>
+        <v>909</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>632</v>
+        <v>1052</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>670</v>
+        <v>1053</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>671</v>
+        <v>1054</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>739</v>
+        <v>1055</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>911</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>695</v>
+        <v>673</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>676</v>
+        <v>695</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>677</v>
+        <v>741</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>816</v>
+        <v>913</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>743</v>
+        <v>679</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>915</v>
+        <v>816</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>685</v>
+        <v>743</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>745</v>
+        <v>685</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>925</v>
+        <v>641</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="D205" s="6" t="s">
-        <v>748</v>
-      </c>
-      <c r="E205" s="3" t="s">
-        <v>750</v>
-      </c>
-      <c r="F205" s="6" t="s">
-        <v>921</v>
+        <v>687</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>924</v>
@@ -8519,809 +8567,844 @@
       <c r="C206" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D206" s="4" t="s">
+      <c r="D206" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="E206" s="3" t="s">
         <v>749</v>
       </c>
-      <c r="E206" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="F206" s="4" t="s">
-        <v>922</v>
+      <c r="F206" s="6" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>697</v>
+        <v>923</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>457</v>
+        <v>745</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>698</v>
+        <v>748</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>703</v>
+        <v>750</v>
       </c>
       <c r="F207" s="4" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="F208" s="4" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>998</v>
+        <v>696</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>999</v>
+        <v>456</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>1000</v>
+        <v>699</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>1001</v>
+        <v>701</v>
       </c>
       <c r="F209" s="4" t="s">
-        <v>1002</v>
+        <v>919</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>926</v>
+        <v>997</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>928</v>
+        <v>998</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>930</v>
+        <v>999</v>
       </c>
       <c r="E210" s="3" t="s">
-        <v>932</v>
+        <v>1000</v>
       </c>
       <c r="F210" s="4" t="s">
-        <v>933</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B211" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C211" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="C211" s="1" t="s">
+      <c r="D211" s="4" t="s">
         <v>929</v>
       </c>
-      <c r="D211" s="4" t="s">
+      <c r="E211" s="3" t="s">
         <v>931</v>
       </c>
-      <c r="E211" s="3" t="s">
-        <v>934</v>
-      </c>
       <c r="F211" s="4" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>937</v>
+        <v>926</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>939</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>942</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>938</v>
-      </c>
-      <c r="F212" s="1" t="s">
-        <v>943</v>
+        <v>928</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="F212" s="4" t="s">
+        <v>934</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>936</v>
       </c>
       <c r="C213" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="D213" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="D213" s="1" t="s">
-        <v>944</v>
-      </c>
       <c r="E213" s="1" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>949</v>
+        <v>935</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>948</v>
+        <v>940</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>950</v>
+        <v>943</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>953</v>
+        <v>948</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>955</v>
+        <v>947</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>958</v>
+        <v>950</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B216" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>954</v>
       </c>
-      <c r="C216" s="1" t="s">
+      <c r="D216" s="1" t="s">
         <v>956</v>
       </c>
-      <c r="D216" s="1" t="s">
-        <v>959</v>
-      </c>
       <c r="E216" s="1" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>961</v>
+        <v>956</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>964</v>
+        <v>958</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>965</v>
+        <v>959</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>966</v>
+        <v>960</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>967</v>
+        <v>961</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>968</v>
+        <v>962</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>977</v>
+        <v>964</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>978</v>
+        <v>965</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>979</v>
+        <v>968</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B220" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="C220" s="1" t="s">
         <v>970</v>
       </c>
-      <c r="C220" s="1" t="s">
-        <v>982</v>
-      </c>
       <c r="D220" s="1" t="s">
-        <v>983</v>
+        <v>978</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>984</v>
+        <v>979</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>985</v>
+        <v>980</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>974</v>
+        <v>981</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>248</v>
+        <v>982</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>346</v>
+        <v>983</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>784</v>
+        <v>984</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>986</v>
+        <v>248</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>987</v>
+        <v>346</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>801</v>
+        <v>783</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>988</v>
+        <v>975</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>989</v>
+        <v>974</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>992</v>
+        <v>985</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>991</v>
+        <v>986</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>990</v>
+        <v>800</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>993</v>
+        <v>987</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>995</v>
+        <v>990</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>996</v>
+        <v>989</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>1012</v>
+        <v>992</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D225" s="6" t="s">
-        <v>1014</v>
+        <v>996</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>993</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>1032</v>
+        <v>994</v>
       </c>
       <c r="F225" s="1" t="s">
-        <v>1033</v>
+        <v>995</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>1016</v>
-      </c>
-      <c r="D226" s="1" t="s">
-        <v>1017</v>
+        <v>1012</v>
+      </c>
+      <c r="D226" s="6" t="s">
+        <v>1013</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="C227" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D227" s="1" t="s">
         <v>1016</v>
       </c>
-      <c r="D227" s="1" t="s">
-        <v>1017</v>
-      </c>
       <c r="E227" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F227" s="1" t="s">
         <v>1034</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>1058</v>
+        <v>1017</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>351</v>
+        <v>1033</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>255</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>1036</v>
+        <v>351</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>1037</v>
+        <v>255</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>1023</v>
+        <v>1058</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1027</v>
+        <v>1020</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1030</v>
+        <v>1021</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>1026</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B232" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C232" s="1" t="s">
         <v>1025</v>
       </c>
-      <c r="C232" s="1" t="s">
-        <v>1028</v>
-      </c>
       <c r="D232" s="1" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>1044</v>
+        <v>1024</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>451</v>
+        <v>1027</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1045</v>
+        <v>1028</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>331</v>
+        <v>1041</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
+        <v>231</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
         <v>232</v>
       </c>
-      <c r="B234" s="1" t="s">
+      <c r="B235" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C235" s="1" t="s">
         <v>1060</v>
       </c>
-      <c r="C234" s="1" t="s">
+      <c r="D235" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E235" s="1" t="s">
         <v>1061</v>
       </c>
-      <c r="D234" s="1" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E234" s="1" t="s">
+      <c r="F235" s="1" t="s">
         <v>1062</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>1063</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B167:E168 B1:E3 B153:E165 B96:E151 B69:E72 B5:E15 B17:E66 B178:E206 B210:E210 B212:E1048576 B75:E89">
+  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E166 B97:E152 B69:E72 B5:E15 B17:E66 B179:E207 B211:E211 B213:E1048576 B75:E89">
+    <cfRule type="cellIs" dxfId="49" priority="52" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B167:E167">
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B171:E172">
+    <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B153:E153">
     <cfRule type="cellIs" dxfId="46" priority="49" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B166:E166">
+  <conditionalFormatting sqref="B173:E173 B174 D174:E174">
     <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B170:E171">
+  <conditionalFormatting sqref="B175:E175 B176 D176:E176">
     <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B152:E152">
+  <conditionalFormatting sqref="B177:E178">
     <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B172:E172 B173 D173:E173">
+  <conditionalFormatting sqref="C176">
     <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B174:E174 B175 D175:E175">
+  <conditionalFormatting sqref="C174">
     <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B176:E177">
+  <conditionalFormatting sqref="B90:E90">
     <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C175">
+  <conditionalFormatting sqref="B91:D93">
     <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C173">
+  <conditionalFormatting sqref="E91:E92">
     <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:E90">
+  <conditionalFormatting sqref="B94:D94 B96:D96">
     <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:D93">
+  <conditionalFormatting sqref="E94 E96">
     <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E92">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:D95">
+  <conditionalFormatting sqref="B67:E68">
     <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E94:E95">
+  <conditionalFormatting sqref="B208:E209">
     <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
+  <conditionalFormatting sqref="B73:D74">
     <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:E68">
+  <conditionalFormatting sqref="E74">
     <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B207:E208">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:D74">
+  <conditionalFormatting sqref="B16:E16">
     <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="B207:E207">
     <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:E16">
+  <conditionalFormatting sqref="B206:E206">
     <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93">
+  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F66 F179:F207 F211 F213:F1048576">
     <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B206:E206">
+  <conditionalFormatting sqref="F167">
     <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B205:E205">
+  <conditionalFormatting sqref="F171:F172">
     <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F167:F168 F1:F3 F153:F165 F96:F151 F69:F72 F5:F15 F75:F89 F17:F66 F178:F206 F210 F212:F1048576">
+  <conditionalFormatting sqref="F153">
     <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F166">
+  <conditionalFormatting sqref="F173:F174">
     <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F170:F171">
+  <conditionalFormatting sqref="F175:F176">
     <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F152">
+  <conditionalFormatting sqref="F177:F178">
     <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F172:F173">
+  <conditionalFormatting sqref="F90">
     <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F174:F175">
+  <conditionalFormatting sqref="F91:F93">
     <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F176:F177">
+  <conditionalFormatting sqref="F94 F96">
     <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90">
+  <conditionalFormatting sqref="F4">
     <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:F93">
+  <conditionalFormatting sqref="F67:F68">
     <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94:F95">
+  <conditionalFormatting sqref="F208:F209">
     <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="F73:F74">
     <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67:F68">
+  <conditionalFormatting sqref="F16">
     <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207:F208">
+  <conditionalFormatting sqref="F207">
     <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:F74">
+  <conditionalFormatting sqref="F206">
     <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+  <conditionalFormatting sqref="B212:E212">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F206">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+  <conditionalFormatting sqref="F212">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F205">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+  <conditionalFormatting sqref="B210:E210">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B211:E211">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+  <conditionalFormatting sqref="F210">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F211">
+  <conditionalFormatting sqref="B170:E170">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B209:E209">
+  <conditionalFormatting sqref="F170">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F209">
+  <conditionalFormatting sqref="B95:D95">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B169:E169">
+  <conditionalFormatting sqref="E95">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F169">
+  <conditionalFormatting sqref="F95">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>